<commit_message>
change to "volume (µl)" in table
</commit_message>
<xml_diff>
--- a/www/Mass_Spec_Preppy_sample_meta_template.xlsx
+++ b/www/Mass_Spec_Preppy_sample_meta_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanmichalik/Desktop/Shiny_Projects/Mass_Spec_Preppy/www/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanmichalik/Desktop/Shiny_Projects/MassSpecPreppy/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9417A9AC-4C47-D14B-9913-1B21B272FE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EEDEF0-6FB3-7846-A9F3-C28CD6E13A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7080" yWindow="3320" windowWidth="26840" windowHeight="15940" xr2:uid="{9C6DEB3A-04B0-994D-AA0B-D6DC73DC01D0}"/>
   </bookViews>
@@ -125,9 +125,6 @@
     <t>samples3</t>
   </si>
   <si>
-    <t>volume</t>
-  </si>
-  <si>
     <t>OT-2 slot</t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>H12</t>
+  </si>
+  <si>
+    <t>volume (µl)</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -522,22 +522,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -856,7 +855,7 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,28 +869,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="4">
@@ -903,379 +902,357 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7">
-        <v>100</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7">
-        <v>100</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="7">
-        <v>100</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7">
-        <v>100</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>34</v>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="7">
-        <v>100</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>35</v>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="7">
-        <v>100</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>36</v>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="7">
-        <v>100</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>37</v>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="7">
-        <v>100</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="7">
-        <v>100</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="7">
-        <v>100</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="7">
-        <v>100</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="7">
-        <v>100</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>38</v>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="7">
-        <v>100</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>39</v>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="7">
-        <v>100</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>40</v>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="7">
-        <v>100</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>41</v>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="7">
-        <v>100</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="7">
-        <v>100</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="E19">
+        <v>100</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="7">
-        <v>100</v>
-      </c>
-      <c r="F20" s="8" t="s">
+      <c r="E20">
+        <v>100</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="7">
-        <v>100</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="E21">
+        <v>100</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="7">
-        <v>100</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>42</v>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="7">
-        <v>100</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>43</v>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="7">
-        <v>100</v>
-      </c>
-      <c r="F24" s="8" t="s">
+      <c r="E24">
+        <v>100</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="9">
+        <v>100</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="10">
-        <v>100</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="4">
@@ -1287,1138 +1264,1072 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="7">
-        <v>100</v>
-      </c>
-      <c r="F27" s="8" t="s">
+      <c r="E27">
+        <v>100</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="7">
-        <v>100</v>
-      </c>
-      <c r="F28" s="8" t="s">
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="7">
-        <v>100</v>
-      </c>
-      <c r="F29" s="8" t="s">
+      <c r="E29">
+        <v>100</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="7">
-        <v>100</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>46</v>
+      <c r="E30">
+        <v>100</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="7">
-        <v>100</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>47</v>
+      <c r="E31">
+        <v>100</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="7">
-        <v>100</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>48</v>
+      <c r="E32">
+        <v>100</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="7">
-        <v>100</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>49</v>
+      <c r="E33">
+        <v>100</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="7">
-        <v>100</v>
-      </c>
-      <c r="F34" s="8" t="s">
+      <c r="E34">
+        <v>100</v>
+      </c>
+      <c r="F34" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="7">
-        <v>100</v>
-      </c>
-      <c r="F35" s="8" t="s">
+      <c r="E35">
+        <v>100</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="7">
-        <v>100</v>
-      </c>
-      <c r="F36" s="8" t="s">
+      <c r="E36">
+        <v>100</v>
+      </c>
+      <c r="F36" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="7">
-        <v>100</v>
-      </c>
-      <c r="F37" s="8" t="s">
+      <c r="E37">
+        <v>100</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E38" s="7">
-        <v>100</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>50</v>
+      <c r="E38">
+        <v>100</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="7">
-        <v>100</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>51</v>
+      <c r="E39">
+        <v>100</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E40" s="7">
-        <v>100</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>52</v>
+      <c r="E40">
+        <v>100</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="7">
-        <v>100</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>53</v>
+      <c r="E41">
+        <v>100</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="7">
-        <v>100</v>
-      </c>
-      <c r="F42" s="8" t="s">
+      <c r="E42">
+        <v>100</v>
+      </c>
+      <c r="F42" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="7">
-        <v>100</v>
-      </c>
-      <c r="F43" s="8" t="s">
+      <c r="E43">
+        <v>100</v>
+      </c>
+      <c r="F43" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="7">
-        <v>100</v>
-      </c>
-      <c r="F44" s="8" t="s">
+      <c r="E44">
+        <v>100</v>
+      </c>
+      <c r="F44" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="7">
-        <v>100</v>
-      </c>
-      <c r="F45" s="8" t="s">
+      <c r="E45">
+        <v>100</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="D46" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="7">
-        <v>100</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>54</v>
+      <c r="E46">
+        <v>100</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E47" s="7">
-        <v>100</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>55</v>
+      <c r="E47">
+        <v>100</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E48" s="7">
-        <v>100</v>
-      </c>
-      <c r="F48" s="8" t="s">
+      <c r="E48">
+        <v>100</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="8"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="9">
+        <v>100</v>
+      </c>
+      <c r="F49" s="10" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="9"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E49" s="10">
-        <v>100</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D50" s="21" t="s">
+      <c r="D50" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E50" s="4">
         <v>100</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="22" t="s">
+      <c r="C51" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D51" s="22" t="s">
+      <c r="D51" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="7">
-        <v>100</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>59</v>
+      <c r="E51">
+        <v>100</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="22" t="s">
+      <c r="C52" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D52" s="22" t="s">
+      <c r="D52" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="7">
-        <v>100</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>60</v>
+      <c r="E52">
+        <v>100</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D53" s="22" t="s">
+      <c r="D53" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="7">
-        <v>100</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>61</v>
+      <c r="E53">
+        <v>100</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="22" t="s">
+      <c r="C54" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D54" s="22" t="s">
+      <c r="D54" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="7">
-        <v>100</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>62</v>
+      <c r="E54">
+        <v>100</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D55" s="22" t="s">
+      <c r="D55" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="7">
-        <v>100</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>63</v>
+      <c r="E55">
+        <v>100</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="22" t="s">
+      <c r="C56" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D56" s="22" t="s">
+      <c r="D56" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E56" s="7">
-        <v>100</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>64</v>
+      <c r="E56">
+        <v>100</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="22" t="s">
+      <c r="C57" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D57" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E57" s="7">
-        <v>100</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>65</v>
+      <c r="E57">
+        <v>100</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="22" t="s">
+      <c r="C58" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="D58" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E58" s="7">
-        <v>100</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>66</v>
+      <c r="E58">
+        <v>100</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="22" t="s">
+      <c r="C59" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="D59" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="7">
-        <v>100</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>67</v>
+      <c r="E59">
+        <v>100</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="6"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="22" t="s">
+      <c r="C60" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D60" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E60" s="7">
-        <v>100</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>68</v>
+      <c r="E60">
+        <v>100</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="22" t="s">
+      <c r="C61" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D61" s="22" t="s">
+      <c r="D61" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E61" s="7">
-        <v>100</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>69</v>
+      <c r="E61">
+        <v>100</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="6"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="22" t="s">
+      <c r="C62" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="D62" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E62" s="7">
-        <v>100</v>
-      </c>
-      <c r="F62" s="8" t="s">
-        <v>70</v>
+      <c r="E62">
+        <v>100</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="6"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="22" t="s">
+      <c r="C63" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="D63" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E63" s="7">
-        <v>100</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>71</v>
+      <c r="E63">
+        <v>100</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="6"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="22" t="s">
+      <c r="C64" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D64" s="22" t="s">
+      <c r="D64" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="7">
-        <v>100</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>72</v>
+      <c r="E64">
+        <v>100</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="6"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="22" t="s">
+      <c r="C65" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D65" s="22" t="s">
+      <c r="D65" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E65" s="7">
-        <v>100</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>73</v>
+      <c r="E65">
+        <v>100</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="6"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="22" t="s">
+      <c r="C66" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D66" s="22" t="s">
+      <c r="D66" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E66" s="7">
-        <v>100</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>74</v>
+      <c r="E66">
+        <v>100</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="6"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="22" t="s">
+      <c r="C67" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D67" s="22" t="s">
+      <c r="D67" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E67" s="7">
-        <v>100</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>75</v>
+      <c r="E67">
+        <v>100</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="6"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="22" t="s">
+      <c r="C68" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D68" s="22" t="s">
+      <c r="D68" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E68" s="7">
-        <v>100</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>76</v>
+      <c r="E68">
+        <v>100</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="6"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="22" t="s">
+      <c r="C69" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D69" s="22" t="s">
+      <c r="D69" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E69" s="7">
-        <v>100</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>77</v>
+      <c r="E69">
+        <v>100</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="6"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="22" t="s">
+      <c r="C70" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D70" s="22" t="s">
+      <c r="D70" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E70" s="7">
-        <v>100</v>
-      </c>
-      <c r="F70" s="8" t="s">
-        <v>78</v>
+      <c r="E70">
+        <v>100</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="6"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="22" t="s">
+      <c r="C71" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D71" s="22" t="s">
+      <c r="D71" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E71" s="7">
-        <v>100</v>
-      </c>
-      <c r="F71" s="8" t="s">
-        <v>79</v>
+      <c r="E71">
+        <v>100</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="6"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="22" t="s">
+      <c r="C72" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="D72" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E72" s="7">
-        <v>100</v>
-      </c>
-      <c r="F72" s="8" t="s">
+      <c r="E72">
+        <v>100</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="8"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E73" s="9">
+        <v>100</v>
+      </c>
+      <c r="F73" s="10" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="9"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D73" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E73" s="10">
-        <v>100</v>
-      </c>
-      <c r="F73" s="11" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
-      <c r="C74" s="18" t="s">
+      <c r="C74" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D74" s="18" t="s">
+      <c r="D74" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E74" s="4">
         <v>100</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="6"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="19" t="s">
+      <c r="C75" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D75" s="19" t="s">
+      <c r="D75" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E75" s="7">
-        <v>100</v>
-      </c>
-      <c r="F75" s="8" t="s">
-        <v>83</v>
+      <c r="E75">
+        <v>100</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="6"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="19" t="s">
+      <c r="C76" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="D76" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E76" s="7">
-        <v>100</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>84</v>
+      <c r="E76">
+        <v>100</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="6"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="19" t="s">
+      <c r="C77" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D77" s="19" t="s">
+      <c r="D77" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E77" s="7">
-        <v>100</v>
-      </c>
-      <c r="F77" s="8" t="s">
-        <v>85</v>
+      <c r="E77">
+        <v>100</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="6"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="19" t="s">
+      <c r="C78" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D78" s="19" t="s">
+      <c r="D78" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E78" s="7">
-        <v>100</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>86</v>
+      <c r="E78">
+        <v>100</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="6"/>
-      <c r="B79" s="7"/>
-      <c r="C79" s="19" t="s">
+      <c r="C79" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="19" t="s">
+      <c r="D79" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E79" s="7">
-        <v>100</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>87</v>
+      <c r="E79">
+        <v>100</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="6"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="19" t="s">
+      <c r="C80" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D80" s="19" t="s">
+      <c r="D80" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E80" s="7">
-        <v>100</v>
-      </c>
-      <c r="F80" s="8" t="s">
-        <v>88</v>
+      <c r="E80">
+        <v>100</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="6"/>
-      <c r="B81" s="7"/>
-      <c r="C81" s="19" t="s">
+      <c r="C81" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D81" s="19" t="s">
+      <c r="D81" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E81" s="7">
-        <v>100</v>
-      </c>
-      <c r="F81" s="8" t="s">
-        <v>89</v>
+      <c r="E81">
+        <v>100</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="6"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="19" t="s">
+      <c r="C82" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D82" s="19" t="s">
+      <c r="D82" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E82" s="7">
-        <v>100</v>
-      </c>
-      <c r="F82" s="8" t="s">
-        <v>90</v>
+      <c r="E82">
+        <v>100</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="6"/>
-      <c r="B83" s="7"/>
-      <c r="C83" s="19" t="s">
+      <c r="C83" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D83" s="19" t="s">
+      <c r="D83" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E83" s="7">
-        <v>100</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>91</v>
+      <c r="E83">
+        <v>100</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="6"/>
-      <c r="B84" s="7"/>
-      <c r="C84" s="19" t="s">
+      <c r="C84" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D84" s="19" t="s">
+      <c r="D84" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E84" s="7">
-        <v>100</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>92</v>
+      <c r="E84">
+        <v>100</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="6"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D85" s="19" t="s">
+      <c r="D85" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E85" s="7">
-        <v>100</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>93</v>
+      <c r="E85">
+        <v>100</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="6"/>
-      <c r="B86" s="7"/>
-      <c r="C86" s="19" t="s">
+      <c r="C86" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D86" s="19" t="s">
+      <c r="D86" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E86" s="7">
-        <v>100</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>94</v>
+      <c r="E86">
+        <v>100</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="6"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="19" t="s">
+      <c r="C87" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D87" s="19" t="s">
+      <c r="D87" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E87" s="7">
-        <v>100</v>
-      </c>
-      <c r="F87" s="8" t="s">
-        <v>95</v>
+      <c r="E87">
+        <v>100</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="6"/>
-      <c r="B88" s="7"/>
-      <c r="C88" s="19" t="s">
+      <c r="C88" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="19" t="s">
+      <c r="D88" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E88" s="7">
-        <v>100</v>
-      </c>
-      <c r="F88" s="8" t="s">
-        <v>96</v>
+      <c r="E88">
+        <v>100</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="6"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="19" t="s">
+      <c r="C89" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D89" s="19" t="s">
+      <c r="D89" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E89" s="7">
-        <v>100</v>
-      </c>
-      <c r="F89" s="8" t="s">
-        <v>97</v>
+      <c r="E89">
+        <v>100</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="6"/>
-      <c r="B90" s="7"/>
-      <c r="C90" s="19" t="s">
+      <c r="C90" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D90" s="19" t="s">
+      <c r="D90" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E90" s="7">
-        <v>100</v>
-      </c>
-      <c r="F90" s="8" t="s">
-        <v>98</v>
+      <c r="E90">
+        <v>100</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="6"/>
-      <c r="B91" s="7"/>
-      <c r="C91" s="19" t="s">
+      <c r="C91" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D91" s="19" t="s">
+      <c r="D91" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E91" s="7">
-        <v>100</v>
-      </c>
-      <c r="F91" s="8" t="s">
-        <v>99</v>
+      <c r="E91">
+        <v>100</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="6"/>
-      <c r="B92" s="7"/>
-      <c r="C92" s="19" t="s">
+      <c r="C92" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D92" s="19" t="s">
+      <c r="D92" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E92" s="7">
-        <v>100</v>
-      </c>
-      <c r="F92" s="8" t="s">
-        <v>100</v>
+      <c r="E92">
+        <v>100</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="6"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="19" t="s">
+      <c r="C93" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D93" s="19" t="s">
+      <c r="D93" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E93" s="7">
-        <v>100</v>
-      </c>
-      <c r="F93" s="8" t="s">
-        <v>101</v>
+      <c r="E93">
+        <v>100</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="6"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="19" t="s">
+      <c r="C94" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D94" s="19" t="s">
+      <c r="D94" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E94" s="7">
-        <v>100</v>
-      </c>
-      <c r="F94" s="8" t="s">
-        <v>102</v>
+      <c r="E94">
+        <v>100</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="6"/>
-      <c r="B95" s="7"/>
-      <c r="C95" s="19" t="s">
+      <c r="C95" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D95" s="19" t="s">
+      <c r="D95" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E95" s="7">
-        <v>100</v>
-      </c>
-      <c r="F95" s="8" t="s">
-        <v>103</v>
+      <c r="E95">
+        <v>100</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="6"/>
-      <c r="B96" s="7"/>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D96" s="19" t="s">
+      <c r="D96" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E96" s="7">
-        <v>100</v>
-      </c>
-      <c r="F96" s="8" t="s">
+      <c r="E96">
+        <v>100</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="8"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D97" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E97" s="9">
+        <v>100</v>
+      </c>
+      <c r="F97" s="10" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="9"/>
-      <c r="B97" s="10"/>
-      <c r="C97" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D97" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E97" s="10">
-        <v>100</v>
-      </c>
-      <c r="F97" s="11" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>